<commit_message>
lekcja 26 pazdziernika 1LOr 2LOr
</commit_message>
<xml_diff>
--- a/2020/LO1Roz/Lekcja_2/payroll.xlsx
+++ b/2020/LO1Roz/Lekcja_2/payroll.xlsx
@@ -14,6 +14,9 @@
   <sheets>
     <sheet name="wynagrodzenia" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">wynagrodzenia!$A$1:$D$31</definedName>
+  </definedNames>
   <calcPr calcId="162913"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -24,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="109" uniqueCount="42">
   <si>
     <t>Do wypłaty</t>
   </si>
@@ -78,9 +81,6 @@
   </si>
   <si>
     <t>Ostrowska Ewa</t>
-  </si>
-  <si>
-    <t xml:space="preserve">przelew </t>
   </si>
   <si>
     <t>Puławska Cecylia</t>
@@ -162,7 +162,7 @@
   <numFmts count="1">
     <numFmt numFmtId="43" formatCode="_-* #,##0.00\ _z_ł_-;\-* #,##0.00\ _z_ł_-;_-* &quot;-&quot;??\ _z_ł_-;_-@_-"/>
   </numFmts>
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -191,6 +191,15 @@
     <font>
       <b/>
       <sz val="14"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -251,7 +260,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -265,9 +274,6 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="2" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -275,6 +281,11 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="43" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Dziesiętny" xfId="1" builtinId="3"/>
@@ -559,17 +570,19 @@
   <dimension ref="A1:J31"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I32" sqref="I32"/>
+      <selection activeCell="J31" sqref="J31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="29.28515625" customWidth="1"/>
-    <col min="3" max="3" width="26.140625" customWidth="1"/>
+    <col min="1" max="1" width="29.28515625" customWidth="1"/>
+    <col min="2" max="2" width="29.28515625" style="12" customWidth="1"/>
+    <col min="3" max="3" width="26.140625" style="12" customWidth="1"/>
     <col min="4" max="4" width="18.85546875" style="1" customWidth="1"/>
     <col min="5" max="5" width="13.5703125" customWidth="1"/>
     <col min="8" max="8" width="10.28515625" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="20" style="1" customWidth="1"/>
+    <col min="9" max="9" width="12.42578125" customWidth="1"/>
+    <col min="10" max="10" width="21.140625" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:10" x14ac:dyDescent="0.25">
@@ -577,7 +590,7 @@
         <v>1</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>2</v>
@@ -590,8 +603,8 @@
       <c r="A2" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>32</v>
+      <c r="B2" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C2" s="5" t="s">
         <v>4</v>
@@ -604,11 +617,11 @@
       <c r="A3" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>32</v>
+      <c r="B3" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C3" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D3" s="6">
         <v>1140.78</v>
@@ -616,10 +629,10 @@
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="4" t="s">
-        <v>33</v>
-      </c>
-      <c r="B4" s="4" t="s">
         <v>32</v>
+      </c>
+      <c r="B4" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C4" s="5" t="s">
         <v>4</v>
@@ -632,8 +645,8 @@
       <c r="A5" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="B5" s="4" t="s">
-        <v>32</v>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C5" s="5" t="s">
         <v>4</v>
@@ -646,11 +659,11 @@
       <c r="A6" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="B6" s="4" t="s">
-        <v>32</v>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C6" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D6" s="6">
         <v>1181.95</v>
@@ -660,11 +673,11 @@
       <c r="A7" s="4" t="s">
         <v>8</v>
       </c>
-      <c r="B7" s="4" t="s">
-        <v>32</v>
+      <c r="B7" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C7" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D7" s="6">
         <v>1036.3000000000002</v>
@@ -674,8 +687,8 @@
       <c r="A8" s="4" t="s">
         <v>9</v>
       </c>
-      <c r="B8" s="4" t="s">
-        <v>32</v>
+      <c r="B8" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>4</v>
@@ -683,22 +696,22 @@
       <c r="D8" s="6">
         <v>412.13000000000005</v>
       </c>
-      <c r="H8" s="5" t="s">
+      <c r="H8" s="2" t="s">
+        <v>37</v>
+      </c>
+      <c r="I8" s="2" t="s">
         <v>38</v>
       </c>
-      <c r="I8" s="5" t="s">
+      <c r="J8" s="3" t="s">
         <v>39</v>
-      </c>
-      <c r="J8" s="7" t="s">
-        <v>40</v>
       </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="B9" s="4" t="s">
-        <v>32</v>
+      <c r="B9" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C9" s="5" t="s">
         <v>4</v>
@@ -706,18 +719,21 @@
       <c r="D9" s="6">
         <v>1135.2700000000002</v>
       </c>
-      <c r="H9" s="8"/>
+      <c r="H9" s="7"/>
       <c r="I9" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J9" s="6"/>
+      <c r="J9" s="6">
+        <f>SUMIFS($D$2:$D$30,$C$2:$C$30,I9)</f>
+        <v>19229.320000000003</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10" s="4" t="s">
+        <v>35</v>
+      </c>
+      <c r="B10" s="5" t="s">
         <v>36</v>
-      </c>
-      <c r="B10" s="4" t="s">
-        <v>37</v>
       </c>
       <c r="C10" s="5" t="s">
         <v>4</v>
@@ -725,18 +741,21 @@
       <c r="D10" s="6">
         <v>1303.6000000000001</v>
       </c>
-      <c r="H10" s="8"/>
+      <c r="H10" s="7"/>
       <c r="I10" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J10" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="J10" s="13">
+        <f>SUMIFS($D$2:$D$30,$C$2:$C$30,I10)</f>
+        <v>14340.439999999999</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B11" s="4" t="s">
-        <v>37</v>
+        <v>33</v>
+      </c>
+      <c r="B11" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C11" s="5" t="s">
         <v>4</v>
@@ -744,96 +763,105 @@
       <c r="D11" s="6">
         <v>2419.0300000000002</v>
       </c>
-      <c r="H11" s="8"/>
-      <c r="I11" s="8"/>
-      <c r="J11" s="9"/>
+      <c r="H11" s="7"/>
+      <c r="I11" s="7"/>
+      <c r="J11" s="8"/>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="4" t="s">
-        <v>32</v>
+      <c r="B12" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C12" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D12" s="6">
         <v>1057.78</v>
       </c>
       <c r="H12" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I12" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J12" s="6"/>
+      <c r="J12" s="6">
+        <f>SUMIFS($D$2:$D$30,$B$2:$B$30,H12,$C$2:$C$30,I12)</f>
+        <v>11680.37</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13" s="4" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="4" t="s">
-        <v>32</v>
+      <c r="B13" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C13" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D13" s="6">
         <v>591.06000000000006</v>
       </c>
       <c r="H13" s="4" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I13" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J13" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="J13" s="6">
+        <f>SUMIFS($D$2:$D$30,$B$2:$B$30,H13,$C$2:$C$30,I13)</f>
+        <v>14340.439999999999</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="B14" s="4" t="s">
-        <v>32</v>
+      <c r="B14" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C14" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D14" s="6">
         <v>701.53</v>
       </c>
-      <c r="H14" s="8"/>
-      <c r="I14" s="8"/>
-      <c r="J14" s="9"/>
+      <c r="H14" s="7"/>
+      <c r="I14" s="7"/>
+      <c r="J14" s="8"/>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15" s="4" t="s">
         <v>14</v>
       </c>
-      <c r="B15" s="4" t="s">
-        <v>32</v>
+      <c r="B15" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C15" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D15" s="6">
         <v>778.30000000000007</v>
       </c>
       <c r="H15" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I15" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="J15" s="6"/>
+      <c r="J15" s="6">
+        <f>SUMIFS($D$2:$D$30,$B$2:$B$30,H15,$C$2:$C$30,I15)</f>
+        <v>7548.95</v>
+      </c>
     </row>
     <row r="16" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A16" s="4" t="s">
         <v>15</v>
       </c>
-      <c r="B16" s="4" t="s">
-        <v>37</v>
+      <c r="B16" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C16" s="5" t="s">
         <v>4</v>
@@ -842,22 +870,25 @@
         <v>1199.3699999999999</v>
       </c>
       <c r="H16" s="4" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="I16" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="J16" s="6"/>
+        <v>29</v>
+      </c>
+      <c r="J16" s="6">
+        <f>SUMIFS($D$2:$D$30,$B$2:$B$30,H16,$C$2:$C$30,I16)</f>
+        <v>0</v>
+      </c>
     </row>
     <row r="17" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A17" s="4" t="s">
         <v>16</v>
       </c>
-      <c r="B17" s="4" t="s">
-        <v>32</v>
+      <c r="B17" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C17" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D17" s="6">
         <v>791.30000000000007</v>
@@ -867,50 +898,56 @@
       <c r="A18" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B18" s="4" t="s">
-        <v>32</v>
+      <c r="B18" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C18" s="5" t="s">
-        <v>18</v>
+        <v>4</v>
       </c>
       <c r="D18" s="6">
         <v>1212.1500000000001</v>
       </c>
-      <c r="H18" s="11" t="s">
-        <v>32</v>
-      </c>
-      <c r="I18" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J18" s="12"/>
+      <c r="H18" s="10" t="s">
+        <v>31</v>
+      </c>
+      <c r="I18" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J18" s="11">
+        <f>AVERAGEIFS($D$2:$D$30,$B$2:$B$30,H18)</f>
+        <v>1040.8324</v>
+      </c>
     </row>
     <row r="19" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A19" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="B19" s="4" t="s">
-        <v>32</v>
+        <v>18</v>
+      </c>
+      <c r="B19" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C19" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D19" s="6">
         <v>1133.9299999999998</v>
       </c>
-      <c r="H19" s="11" t="s">
-        <v>37</v>
-      </c>
-      <c r="I19" s="11" t="s">
-        <v>42</v>
-      </c>
-      <c r="J19" s="12"/>
+      <c r="H19" s="10" t="s">
+        <v>36</v>
+      </c>
+      <c r="I19" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="J19" s="11">
+        <f>AVERAGEIFS($D$2:$D$30,$B$2:$B$30,H19)</f>
+        <v>1887.2375</v>
+      </c>
     </row>
     <row r="20" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A20" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="B20" s="4" t="s">
-        <v>32</v>
+        <v>19</v>
+      </c>
+      <c r="B20" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C20" s="5" t="s">
         <v>4</v>
@@ -921,13 +958,13 @@
     </row>
     <row r="21" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A21" s="4" t="s">
-        <v>21</v>
-      </c>
-      <c r="B21" s="4" t="s">
-        <v>32</v>
+        <v>20</v>
+      </c>
+      <c r="B21" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C21" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D21" s="6">
         <v>2053.23</v>
@@ -935,13 +972,13 @@
     </row>
     <row r="22" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A22" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="B22" s="4" t="s">
-        <v>32</v>
+        <v>21</v>
+      </c>
+      <c r="B22" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C22" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D22" s="6">
         <v>1036.3000000000002</v>
@@ -949,10 +986,10 @@
     </row>
     <row r="23" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A23" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B23" s="4" t="s">
-        <v>32</v>
+        <v>22</v>
+      </c>
+      <c r="B23" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C23" s="5" t="s">
         <v>4</v>
@@ -963,10 +1000,10 @@
     </row>
     <row r="24" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A24" s="4" t="s">
-        <v>24</v>
-      </c>
-      <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>23</v>
+      </c>
+      <c r="B24" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C24" s="5" t="s">
         <v>4</v>
@@ -977,10 +1014,10 @@
     </row>
     <row r="25" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A25" s="4" t="s">
-        <v>35</v>
-      </c>
-      <c r="B25" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
+      </c>
+      <c r="B25" s="5" t="s">
+        <v>36</v>
       </c>
       <c r="C25" s="5" t="s">
         <v>4</v>
@@ -991,13 +1028,13 @@
     </row>
     <row r="26" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A26" s="4" t="s">
-        <v>25</v>
-      </c>
-      <c r="B26" s="4" t="s">
-        <v>32</v>
+        <v>24</v>
+      </c>
+      <c r="B26" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C26" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D26" s="6">
         <v>1135.2700000000002</v>
@@ -1005,13 +1042,13 @@
     </row>
     <row r="27" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A27" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B27" s="4" t="s">
-        <v>32</v>
+        <v>25</v>
+      </c>
+      <c r="B27" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C27" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D27" s="6">
         <v>743.30000000000007</v>
@@ -1019,10 +1056,10 @@
     </row>
     <row r="28" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A28" s="4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B28" s="4" t="s">
-        <v>32</v>
+        <v>26</v>
+      </c>
+      <c r="B28" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C28" s="5" t="s">
         <v>4</v>
@@ -1033,13 +1070,13 @@
     </row>
     <row r="29" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A29" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="B29" s="4" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+      <c r="B29" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C29" s="5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="D29" s="6">
         <v>959.41000000000008</v>
@@ -1047,10 +1084,10 @@
     </row>
     <row r="30" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A30" s="4" t="s">
-        <v>29</v>
-      </c>
-      <c r="B30" s="4" t="s">
-        <v>32</v>
+        <v>28</v>
+      </c>
+      <c r="B30" s="5" t="s">
+        <v>31</v>
       </c>
       <c r="C30" s="5" t="s">
         <v>4</v>
@@ -1060,8 +1097,12 @@
       </c>
     </row>
     <row r="31" spans="1:10" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="C31" s="10" t="s">
-        <v>41</v>
+      <c r="C31" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="D31" s="14">
+        <f>SUM(D2:D30)</f>
+        <v>33569.760000000002</v>
       </c>
     </row>
   </sheetData>

</xml_diff>